<commit_message>
-Split data engineering and data analysis
</commit_message>
<xml_diff>
--- a/Output/Iterations.xlsx
+++ b/Output/Iterations.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="44">
   <si>
     <t>TileXSize</t>
   </si>
@@ -128,45 +128,6 @@
   </si>
   <si>
     <t>StephB</t>
-  </si>
-  <si>
-    <t>303112001</t>
-  </si>
-  <si>
-    <t>404000100</t>
-  </si>
-  <si>
-    <t>404223002</t>
-  </si>
-  <si>
-    <t>303334003</t>
-  </si>
-  <si>
-    <t>404113101</t>
-  </si>
-  <si>
-    <t>303221202</t>
-  </si>
-  <si>
-    <t>304420003</t>
-  </si>
-  <si>
-    <t>404113001</t>
-  </si>
-  <si>
-    <t>324332103</t>
-  </si>
-  <si>
-    <t>505122002</t>
-  </si>
-  <si>
-    <t>304223302</t>
-  </si>
-  <si>
-    <t>303120402</t>
-  </si>
-  <si>
-    <t>323341324</t>
   </si>
   <si>
     <t>Grasshopper</t>
@@ -626,14 +587,14 @@
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="1">
+        <v>303112001</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="C2" s="1">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="E2" s="1">
         <v>2</v>
@@ -835,7 +796,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E5" s="1">
         <v>2</v>
@@ -1037,7 +998,7 @@
         <v>3</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="E8" s="1">
         <v>2</v>
@@ -1239,7 +1200,7 @@
         <v>0</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="E11" s="1">
         <v>0</v>
@@ -1307,7 +1268,7 @@
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E12" s="1">
         <v>0</v>
@@ -1375,7 +1336,7 @@
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="E13" s="1">
         <v>0</v>
@@ -1442,14 +1403,14 @@
       <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>39</v>
+      <c r="B14" s="1">
+        <v>404000100</v>
       </c>
       <c r="C14" s="1">
         <v>3</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="E14" s="1">
         <v>2</v>
@@ -1651,7 +1612,7 @@
         <v>2</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="E17" s="1">
         <v>2</v>
@@ -1853,7 +1814,7 @@
         <v>0</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="E20" s="1">
         <v>0</v>
@@ -1921,7 +1882,7 @@
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E21" s="1">
         <v>0</v>
@@ -1989,7 +1950,7 @@
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="E22" s="1">
         <v>0</v>
@@ -2056,14 +2017,14 @@
       <c r="A23" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>40</v>
+      <c r="B23" s="1">
+        <v>404223002</v>
       </c>
       <c r="C23" s="1">
         <v>2</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="E23" s="1">
         <v>2</v>
@@ -2265,7 +2226,7 @@
         <v>3</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E26" s="1">
         <v>2</v>
@@ -2467,7 +2428,7 @@
         <v>1</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="E29" s="1">
         <v>2</v>
@@ -2669,7 +2630,7 @@
         <v>0</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="E32" s="1">
         <v>0</v>
@@ -2737,7 +2698,7 @@
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E33" s="1">
         <v>0</v>
@@ -2805,7 +2766,7 @@
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="E34" s="1">
         <v>0</v>
@@ -2872,14 +2833,14 @@
       <c r="A35" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>41</v>
+      <c r="B35" s="1">
+        <v>303334003</v>
       </c>
       <c r="C35" s="1">
         <v>1</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="E35" s="1">
         <v>2</v>
@@ -3081,7 +3042,7 @@
         <v>3</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E38" s="1">
         <v>2</v>
@@ -3283,7 +3244,7 @@
         <v>2</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="E41" s="1">
         <v>2</v>
@@ -3485,7 +3446,7 @@
         <v>0</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="E44" s="1">
         <v>0</v>
@@ -3553,7 +3514,7 @@
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E45" s="1">
         <v>0</v>
@@ -3621,7 +3582,7 @@
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="E46" s="1">
         <v>0</v>
@@ -3688,14 +3649,14 @@
       <c r="A47" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>42</v>
+      <c r="B47" s="1">
+        <v>404113101</v>
       </c>
       <c r="C47" s="1">
         <v>2</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="E47" s="1">
         <v>2</v>
@@ -3897,7 +3858,7 @@
         <v>1</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E50" s="1">
         <v>2</v>
@@ -4099,7 +4060,7 @@
         <v>3</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="E53" s="1">
         <v>2</v>
@@ -4301,7 +4262,7 @@
         <v>0</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="E56" s="1">
         <v>0</v>
@@ -4369,7 +4330,7 @@
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E57" s="1">
         <v>0</v>
@@ -4437,7 +4398,7 @@
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="E58" s="1">
         <v>0</v>
@@ -4504,14 +4465,14 @@
       <c r="A59" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B59" s="1" t="s">
-        <v>43</v>
+      <c r="B59" s="1">
+        <v>303221202</v>
       </c>
       <c r="C59" s="1">
         <v>3</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="E59" s="1">
         <v>2</v>
@@ -4713,7 +4674,7 @@
         <v>2</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E62" s="1">
         <v>2</v>
@@ -4915,7 +4876,7 @@
         <v>1</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="E65" s="1">
         <v>2</v>
@@ -5117,7 +5078,7 @@
         <v>0</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="E68" s="1">
         <v>0</v>
@@ -5185,7 +5146,7 @@
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E69" s="1">
         <v>0</v>
@@ -5253,7 +5214,7 @@
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
       <c r="D70" s="1" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="E70" s="1">
         <v>0</v>
@@ -5320,14 +5281,14 @@
       <c r="A71" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B71" s="1" t="s">
-        <v>44</v>
+      <c r="B71" s="1">
+        <v>304420003</v>
       </c>
       <c r="C71" s="1">
         <v>1</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="E71" s="1">
         <v>2</v>
@@ -5526,7 +5487,7 @@
         <v>2</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E74" s="1">
         <v>2</v>
@@ -5728,7 +5689,7 @@
         <v>3</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="E77" s="1">
         <v>2</v>
@@ -5930,7 +5891,7 @@
         <v>0</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="E80" s="1">
         <v>0</v>
@@ -5998,7 +5959,7 @@
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
       <c r="D81" s="1" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E81" s="1">
         <v>0</v>
@@ -6066,7 +6027,7 @@
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
       <c r="D82" s="1" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="E82" s="1">
         <v>0</v>
@@ -6133,14 +6094,14 @@
       <c r="A83" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B83" s="1" t="s">
-        <v>45</v>
+      <c r="B83" s="1">
+        <v>404113001</v>
       </c>
       <c r="C83" s="1">
         <v>3</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="E83" s="1">
         <v>2</v>
@@ -6342,7 +6303,7 @@
         <v>1</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E86" s="1">
         <v>2</v>
@@ -6544,7 +6505,7 @@
         <v>2</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="E89" s="1">
         <v>2</v>
@@ -6746,7 +6707,7 @@
         <v>0</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="E92" s="1">
         <v>0</v>
@@ -6814,7 +6775,7 @@
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
       <c r="D93" s="1" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E93" s="1">
         <v>0</v>
@@ -6882,7 +6843,7 @@
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
       <c r="D94" s="1" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="E94" s="1">
         <v>0</v>
@@ -6949,14 +6910,14 @@
       <c r="A95" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B95" s="1" t="s">
-        <v>46</v>
+      <c r="B95" s="1">
+        <v>324332103</v>
       </c>
       <c r="C95" s="1">
         <v>2</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="E95" s="1">
         <v>2</v>
@@ -7158,7 +7119,7 @@
         <v>3</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E98" s="1">
         <v>2</v>
@@ -7360,7 +7321,7 @@
         <v>1</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="E101" s="1">
         <v>2</v>
@@ -7562,7 +7523,7 @@
         <v>0</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="E104" s="1">
         <v>0</v>
@@ -7630,7 +7591,7 @@
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
       <c r="D105" s="1" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E105" s="1">
         <v>0</v>
@@ -7698,7 +7659,7 @@
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
       <c r="D106" s="1" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="E106" s="1">
         <v>0</v>
@@ -7765,14 +7726,14 @@
       <c r="A107" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B107" s="1" t="s">
-        <v>47</v>
+      <c r="B107" s="1">
+        <v>505122002</v>
       </c>
       <c r="C107" s="1">
         <v>1</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="E107" s="1">
         <v>2</v>
@@ -7971,7 +7932,7 @@
         <v>3</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E110" s="1">
         <v>2</v>
@@ -8173,7 +8134,7 @@
         <v>2</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="E113" s="1">
         <v>2</v>
@@ -8375,7 +8336,7 @@
         <v>0</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="E116" s="1">
         <v>0</v>
@@ -8443,7 +8404,7 @@
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
       <c r="D117" s="1" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E117" s="1">
         <v>0</v>
@@ -8511,7 +8472,7 @@
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
       <c r="D118" s="1" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="E118" s="1">
         <v>0</v>
@@ -8578,14 +8539,14 @@
       <c r="A119" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B119" s="1" t="s">
-        <v>48</v>
+      <c r="B119" s="1">
+        <v>304223302</v>
       </c>
       <c r="C119" s="1">
         <v>2</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="E119" s="1">
         <v>2</v>
@@ -8787,7 +8748,7 @@
         <v>1</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E122" s="1">
         <v>2</v>
@@ -8989,7 +8950,7 @@
         <v>3</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="E125" s="1">
         <v>2</v>
@@ -9191,7 +9152,7 @@
         <v>0</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="E128" s="1">
         <v>0</v>
@@ -9259,7 +9220,7 @@
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
       <c r="D129" s="1" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E129" s="1">
         <v>0</v>
@@ -9327,7 +9288,7 @@
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
       <c r="D130" s="1" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="E130" s="1">
         <v>0</v>
@@ -9394,14 +9355,14 @@
       <c r="A131" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B131" s="1" t="s">
-        <v>49</v>
+      <c r="B131" s="1">
+        <v>303120402</v>
       </c>
       <c r="C131" s="1">
         <v>3</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="E131" s="1">
         <v>2</v>
@@ -9603,7 +9564,7 @@
         <v>2</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E134" s="1">
         <v>2</v>
@@ -9805,7 +9766,7 @@
         <v>1</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="E137" s="1">
         <v>2</v>
@@ -10007,7 +9968,7 @@
         <v>0</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="E140" s="1">
         <v>0</v>
@@ -10075,7 +10036,7 @@
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
       <c r="D141" s="1" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E141" s="1">
         <v>0</v>
@@ -10143,7 +10104,7 @@
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
       <c r="D142" s="1" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="E142" s="1">
         <v>0</v>
@@ -10210,14 +10171,14 @@
       <c r="A143" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B143" s="1" t="s">
-        <v>50</v>
+      <c r="B143" s="1">
+        <v>323341324</v>
       </c>
       <c r="C143" s="1">
         <v>1</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="E143" s="1">
         <v>2</v>
@@ -10419,7 +10380,7 @@
         <v>2</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E146" s="1">
         <v>2</v>
@@ -10621,7 +10582,7 @@
         <v>3</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="E149" s="1">
         <v>2</v>
@@ -10820,7 +10781,7 @@
         <v>0</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="E152" s="1">
         <v>0</v>
@@ -10888,7 +10849,7 @@
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
       <c r="D153" s="1" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E153" s="1">
         <v>0</v>
@@ -10956,7 +10917,7 @@
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
       <c r="D154" s="1" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="E154" s="1">
         <v>0</v>
@@ -11023,14 +10984,14 @@
       <c r="A155" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B155" s="1" t="s">
-        <v>40</v>
+      <c r="B155" s="1">
+        <v>404223002</v>
       </c>
       <c r="C155" s="1">
         <v>3</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="E155" s="1">
         <v>2</v>
@@ -11232,7 +11193,7 @@
         <v>1</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E158" s="1">
         <v>2</v>
@@ -11434,7 +11395,7 @@
         <v>2</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="E161" s="1">
         <v>2</v>
@@ -11636,7 +11597,7 @@
         <v>0</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="E164" s="1">
         <v>0</v>
@@ -11704,7 +11665,7 @@
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
       <c r="D165" s="1" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E165" s="1">
         <v>0</v>
@@ -11772,7 +11733,7 @@
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
       <c r="D166" s="1" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="E166" s="1">
         <v>0</v>

</xml_diff>

<commit_message>
-Graphic by software level
</commit_message>
<xml_diff>
--- a/Output/Iterations.xlsx
+++ b/Output/Iterations.xlsx
@@ -588,7 +588,7 @@
         <v>24</v>
       </c>
       <c r="B2" s="1">
-        <v>303112001</v>
+        <v>30311200232</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
@@ -1404,7 +1404,7 @@
         <v>25</v>
       </c>
       <c r="B14" s="1">
-        <v>404000100</v>
+        <v>40400010341</v>
       </c>
       <c r="C14" s="1">
         <v>3</v>
@@ -2018,7 +2018,7 @@
         <v>26</v>
       </c>
       <c r="B23" s="1">
-        <v>404223002</v>
+        <v>40422300343</v>
       </c>
       <c r="C23" s="1">
         <v>2</v>
@@ -2834,7 +2834,7 @@
         <v>27</v>
       </c>
       <c r="B35" s="1">
-        <v>303334003</v>
+        <v>30333400334</v>
       </c>
       <c r="C35" s="1">
         <v>1</v>
@@ -3650,7 +3650,7 @@
         <v>28</v>
       </c>
       <c r="B47" s="1">
-        <v>404113101</v>
+        <v>40411310242</v>
       </c>
       <c r="C47" s="1">
         <v>2</v>
@@ -4466,7 +4466,7 @@
         <v>29</v>
       </c>
       <c r="B59" s="1">
-        <v>303221202</v>
+        <v>30322120232</v>
       </c>
       <c r="C59" s="1">
         <v>3</v>
@@ -5282,7 +5282,7 @@
         <v>30</v>
       </c>
       <c r="B71" s="1">
-        <v>304420003</v>
+        <v>30442000340</v>
       </c>
       <c r="C71" s="1">
         <v>1</v>
@@ -6095,7 +6095,7 @@
         <v>31</v>
       </c>
       <c r="B83" s="1">
-        <v>404113001</v>
+        <v>40411300343</v>
       </c>
       <c r="C83" s="1">
         <v>3</v>
@@ -6911,7 +6911,7 @@
         <v>32</v>
       </c>
       <c r="B95" s="1">
-        <v>324332103</v>
+        <v>32433210332</v>
       </c>
       <c r="C95" s="1">
         <v>2</v>
@@ -7727,7 +7727,7 @@
         <v>33</v>
       </c>
       <c r="B107" s="1">
-        <v>505122002</v>
+        <v>50512200352</v>
       </c>
       <c r="C107" s="1">
         <v>1</v>
@@ -8540,7 +8540,7 @@
         <v>34</v>
       </c>
       <c r="B119" s="1">
-        <v>304223302</v>
+        <v>30422330343</v>
       </c>
       <c r="C119" s="1">
         <v>2</v>
@@ -9356,7 +9356,7 @@
         <v>35</v>
       </c>
       <c r="B131" s="1">
-        <v>303120402</v>
+        <v>30312040334</v>
       </c>
       <c r="C131" s="1">
         <v>3</v>
@@ -10172,7 +10172,7 @@
         <v>36</v>
       </c>
       <c r="B143" s="1">
-        <v>323341324</v>
+        <v>32334132322</v>
       </c>
       <c r="C143" s="1">
         <v>1</v>
@@ -10985,7 +10985,7 @@
         <v>37</v>
       </c>
       <c r="B155" s="1">
-        <v>404223002</v>
+        <v>40422300343</v>
       </c>
       <c r="C155" s="1">
         <v>3</v>

</xml_diff>